<commit_message>
Setup ACF Json Sync - Added Course Meta data
Under Custom Fields Page, next to trash you will see a sync option.
Click that to sync these json files.
</commit_message>
<xml_diff>
--- a/QELI Course metadata.xlsx
+++ b/QELI Course metadata.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <workbookPr autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="41400" yWindow="2920" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Field Group</t>
   </si>
@@ -91,9 +99,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Repeater? For collapsible location and date details</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -175,27 +180,52 @@
     <t>Repeater: Case study custom post</t>
   </si>
   <si>
-    <t>Custom post or page depending on usage frequency</t>
+    <t>Changed to Multiselecter post object</t>
+  </si>
+  <si>
+    <t>Moved into Location Reaptor</t>
+  </si>
+  <si>
+    <t>post_tag?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <name val="Arial"/>
     </font>
-    <font/>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -203,7 +233,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -237,269 +267,767 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+  <cellStyleXfs count="83">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2" applyFill="1">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="3">
-      <alignment/>
-    </xf>
-    <xf applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="83">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="22.57"/>
-    <col min="2" customWidth="1" max="2" width="27.71"/>
-    <col min="3" customWidth="1" max="3" width="62.86"/>
-    <col min="4" customWidth="1" max="4" width="42.43"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="62.83203125" customWidth="1"/>
+    <col min="4" max="4" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c t="s" s="1" r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c t="s" s="2" r="A2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="B2">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="3" r="C2">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c t="s" s="2" r="B3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="3" r="C3">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
-      <c t="s" s="2" r="B4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="3" r="C4">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c t="s" s="2" r="B5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="3" r="C5">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6">
-      <c t="s" s="2" r="B6">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="3" r="C6">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7">
-      <c t="s" s="2" r="B7">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="3" r="C7">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8">
-      <c t="s" s="2" r="B8">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="3" r="C8">
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10">
-      <c t="s" s="2" r="A10">
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="2" r="B10">
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="3" r="C10">
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11">
-      <c t="s" s="2" r="B11">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="3" r="C11">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12">
-      <c t="s" s="4" r="B12">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c t="s" s="5" r="C12">
+      <c r="C12" s="5" t="s">
         <v>25</v>
       </c>
-      <c t="s" s="3" r="D12">
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13">
-      <c t="s" s="4" r="B13">
+      <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
-      <c t="s" s="5" r="C13">
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14">
-      <c t="s" s="2" r="B14">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c t="s" s="3" r="C14">
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B15" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15">
-      <c t="s" s="2" r="B15">
+      <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
-      <c t="s" s="3" r="C15">
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16">
-      <c t="s" s="2" r="B16">
+      <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
-      <c t="s" s="3" r="C16">
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17">
-      <c t="s" s="2" r="B17">
+      <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
-      <c t="s" s="3" r="C17">
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18">
-      <c t="s" s="2" r="B18">
+      <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
-      <c t="s" s="3" r="C18">
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20">
-      <c t="s" s="2" r="A20">
+      <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
-      <c t="s" s="2" r="B20">
+      <c r="C20" s="3" t="s">
         <v>40</v>
       </c>
-      <c t="s" s="3" r="C20">
+      <c r="D20" s="3" t="s">
         <v>41</v>
       </c>
-      <c t="s" s="3" r="D20">
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21">
-      <c t="s" s="2" r="B21">
+      <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
-      <c t="s" s="3" r="C21">
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22">
-      <c t="s" s="2" r="B22">
+      <c r="C22" s="6" t="s">
         <v>45</v>
       </c>
-      <c t="s" s="6" r="C22">
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B23" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23">
-      <c t="s" s="2" r="B23">
+      <c r="C23" s="3" t="s">
         <v>47</v>
       </c>
-      <c t="s" s="3" r="C23">
+      <c r="D23" s="3" t="s">
         <v>48</v>
       </c>
-      <c t="s" s="3" r="D23">
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B24" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24">
-      <c t="s" s="2" r="B24">
+      <c r="C24" s="3" t="s">
         <v>50</v>
       </c>
-      <c t="s" s="3" r="C24">
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="B25" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25">
-      <c t="s" s="2" r="B25">
+      <c r="C25" s="3" t="s">
         <v>52</v>
       </c>
-      <c t="s" s="3" r="C25">
+      <c r="D25" t="s">
         <v>53</v>
       </c>
-      <c t="s" s="3" r="D25">
-        <v>54</v>
-      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>